<commit_message>
Plot updated with wishbone generation
</commit_message>
<xml_diff>
--- a/input/Excel_Input_Example.xlsx
+++ b/input/Excel_Input_Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonnyjamison/Desktop/GitHub/KinematicsViewer/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321F6DD5-540D-BB47-AFFC-23992DD9E566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9B6DBE-43CB-8C4A-AA6B-A191DC990A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14500" windowHeight="16080" xr2:uid="{F5DF7F60-5ADB-E54E-BD89-C241984632A6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23700" windowHeight="16080" xr2:uid="{F5DF7F60-5ADB-E54E-BD89-C241984632A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -468,50 +468,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>88899</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>148646</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8FDAFA3-AE1A-CF63-0DDA-8DE61683FCA6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="1790699"/>
-          <a:ext cx="4800600" cy="3717347"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
@@ -585,6 +541,50 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>34925</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>132291</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>158020</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>5820</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD1D03BC-634B-9511-4A7E-E1A5AD6D91BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="34925" y="1799166"/>
+          <a:ext cx="4726845" cy="3445404"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -889,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7443EB16-B5C6-1841-A7F8-5FBC1A2937AD}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="96" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>